<commit_message>
Netzplan Formeln in 01_Netzplan_Übung1.xlsx
</commit_message>
<xml_diff>
--- a/Übungen/01_Netzplan_Übung1.xlsx
+++ b/Übungen/01_Netzplan_Übung1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle2" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="44">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -35,6 +35,15 @@
     <t xml:space="preserve">D</t>
   </si>
   <si>
+    <t xml:space="preserve">FAZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=</t>
+  </si>
+  <si>
+    <t xml:space="preserve">größte FEZ der Vorgänger</t>
+  </si>
+  <si>
     <t xml:space="preserve">A</t>
   </si>
   <si>
@@ -47,39 +56,57 @@
     <t xml:space="preserve">C</t>
   </si>
   <si>
+    <t xml:space="preserve">FEZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAZ + Dauer</t>
+  </si>
+  <si>
     <t xml:space="preserve">F</t>
   </si>
   <si>
+    <t xml:space="preserve">SEZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kleinste SAZ der Nachfolger</t>
+  </si>
+  <si>
     <t xml:space="preserve">E</t>
   </si>
   <si>
+    <t xml:space="preserve">GP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEZ – Dauer</t>
+  </si>
+  <si>
     <t xml:space="preserve">H</t>
   </si>
   <si>
+    <t xml:space="preserve">SEZ – FEZ = SAZ - FAZ</t>
+  </si>
+  <si>
     <t xml:space="preserve">G</t>
   </si>
   <si>
+    <t xml:space="preserve">kleinste FAZ der Nachfolger – FEZ</t>
+  </si>
+  <si>
     <t xml:space="preserve">I</t>
   </si>
   <si>
-    <t xml:space="preserve">FAZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FEZ</t>
-  </si>
-  <si>
     <t xml:space="preserve">← Früheste</t>
   </si>
   <si>
     <t xml:space="preserve">← ID</t>
   </si>
   <si>
-    <t xml:space="preserve">GP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FP</t>
-  </si>
-  <si>
     <t xml:space="preserve">← Dauer &amp; Puffer:</t>
   </si>
   <si>
@@ -93,12 +120,6 @@
   </si>
   <si>
     <t xml:space="preserve">Freier Puffer bis zum nächsten Arbeitspaket</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEZ</t>
   </si>
   <si>
     <t xml:space="preserve">← Späteste</t>
@@ -138,9 +159,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -227,14 +247,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCCCCCC"/>
-        <bgColor rgb="FFCCCCFF"/>
+        <fgColor rgb="FFFDD835"/>
+        <bgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFDD835"/>
-        <bgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -251,14 +271,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF57C00"/>
-        <bgColor rgb="FFFF9900"/>
+        <fgColor rgb="FF43A047"/>
+        <bgColor rgb="FF808080"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF43A047"/>
-        <bgColor rgb="FF808080"/>
+        <fgColor rgb="FFF57C00"/>
+        <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
     <fill>
@@ -303,6 +323,13 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="hair"/>
       <right/>
       <top style="hair"/>
@@ -314,13 +341,6 @@
       <right style="hair"/>
       <top style="hair"/>
       <bottom style="hair"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -384,7 +404,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -405,15 +425,23 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -421,40 +449,48 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -471,14 +507,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1062,8 +1090,8 @@
   </sheetPr>
   <dimension ref="A1:AD44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="1" sqref="P9:R12 A12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V21" activeCellId="0" sqref="V21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.84765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1091,15 +1119,21 @@
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
+      <c r="O1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
       <c r="X1" s="4"/>
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
@@ -1110,35 +1144,49 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="8"/>
+      <c r="B2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="10"/>
       <c r="H2" s="1" t="n">
         <v>6</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
+      <c r="K2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="11"/>
+      <c r="M2" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
       <c r="X2" s="4"/>
       <c r="Y2" s="4"/>
       <c r="Z2" s="4"/>
@@ -1149,31 +1197,43 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
+        <v>9</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
       <c r="H3" s="1" t="n">
         <v>7</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
+      <c r="K3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="O3" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
       <c r="Z3" s="4"/>
@@ -1184,31 +1244,47 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
       <c r="H4" s="1" t="n">
         <v>4</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
-      <c r="W4" s="4"/>
+      <c r="K4" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
       <c r="X4" s="4"/>
       <c r="Y4" s="4"/>
       <c r="Z4" s="4"/>
@@ -1219,36 +1295,46 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
       <c r="H5" s="1" t="n">
         <v>9</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
+      <c r="K5" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="11"/>
+      <c r="M5" s="16" t="s">
+        <v>14</v>
+      </c>
       <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-      <c r="T5" s="4"/>
-      <c r="U5" s="4"/>
-      <c r="V5" s="4"/>
-      <c r="W5" s="4"/>
+      <c r="O5" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
       <c r="X5" s="4"/>
       <c r="Y5" s="4"/>
       <c r="Z5" s="4"/>
@@ -1259,18 +1345,18 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
+        <v>13</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
       <c r="H6" s="1" t="n">
         <v>3</v>
       </c>
@@ -1280,15 +1366,21 @@
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
-      <c r="U6" s="4"/>
-      <c r="V6" s="4"/>
-      <c r="W6" s="4"/>
+      <c r="O6" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q6" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="R6" s="21"/>
+      <c r="S6" s="21"/>
+      <c r="T6" s="21"/>
+      <c r="U6" s="21"/>
+      <c r="V6" s="21"/>
+      <c r="W6" s="21"/>
       <c r="X6" s="4"/>
       <c r="Y6" s="4"/>
       <c r="Z6" s="4"/>
@@ -1299,20 +1391,20 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
+        <v>23</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
       <c r="H7" s="1" t="n">
         <v>3</v>
       </c>
@@ -1341,18 +1433,18 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
+        <v>21</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
       <c r="H8" s="1" t="n">
         <v>7</v>
       </c>
@@ -1381,16 +1473,16 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
+        <v>25</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
       <c r="H9" s="1" t="n">
         <v>9</v>
       </c>
@@ -1477,142 +1569,226 @@
       <c r="AD11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11" t="n">
+      <c r="A12" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="13"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="12" t="n">
+        <f aca="false">A12+A14</f>
+        <v>6</v>
+      </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="13"/>
+      <c r="F12" s="5" t="n">
+        <f aca="false">C12</f>
+        <v>6</v>
+      </c>
+      <c r="G12" s="11"/>
+      <c r="H12" s="12" t="n">
+        <f aca="false">F12+F14</f>
+        <v>13</v>
+      </c>
       <c r="I12" s="4"/>
       <c r="O12" s="4"/>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="13"/>
+      <c r="P12" s="5" t="n">
+        <f aca="false">H12</f>
+        <v>13</v>
+      </c>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="12" t="n">
+        <f aca="false">P12+P14</f>
+        <v>16</v>
+      </c>
       <c r="S12" s="4"/>
       <c r="T12" s="4"/>
-      <c r="U12" s="11"/>
-      <c r="V12" s="12"/>
-      <c r="W12" s="13"/>
+      <c r="U12" s="5" t="n">
+        <f aca="false">MAX(R12,R18)</f>
+        <v>26</v>
+      </c>
+      <c r="V12" s="11"/>
+      <c r="W12" s="12" t="n">
+        <f aca="false">U12+U14</f>
+        <v>29</v>
+      </c>
       <c r="X12" s="4"/>
       <c r="Y12" s="4"/>
-      <c r="Z12" s="11"/>
-      <c r="AA12" s="12"/>
-      <c r="AB12" s="13"/>
+      <c r="Z12" s="5" t="n">
+        <f aca="false">W12</f>
+        <v>29</v>
+      </c>
+      <c r="AA12" s="11"/>
+      <c r="AB12" s="12" t="n">
+        <f aca="false">Z12+Z14</f>
+        <v>38</v>
+      </c>
       <c r="AC12" s="4"/>
       <c r="AD12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
+      <c r="A13" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
-      <c r="F13" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
+      <c r="F13" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
       <c r="I13" s="4"/>
       <c r="O13" s="4"/>
-      <c r="P13" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="14"/>
+      <c r="P13" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
       <c r="S13" s="4"/>
       <c r="T13" s="4"/>
-      <c r="U13" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="V13" s="14"/>
-      <c r="W13" s="14"/>
+      <c r="U13" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="V13" s="15"/>
+      <c r="W13" s="15"/>
       <c r="X13" s="4"/>
       <c r="Y13" s="4"/>
-      <c r="Z13" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA13" s="14"/>
-      <c r="AB13" s="14"/>
+      <c r="Z13" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA13" s="15"/>
+      <c r="AB13" s="15"/>
       <c r="AC13" s="4"/>
       <c r="AD13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="15" t="n">
+      <c r="A14" s="17" t="n">
         <f aca="false">H2</f>
         <v>6</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="15" t="n">
+      <c r="B14" s="18" t="n">
+        <f aca="false">C15-C12</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="19" t="n">
+        <f aca="false">MIN(F12,F18)-C12</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="22"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="17" t="n">
         <f aca="false">H3</f>
         <v>7</v>
       </c>
-      <c r="G14" s="16"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="19"/>
-      <c r="P14" s="15" t="n">
+      <c r="G14" s="18" t="n">
+        <f aca="false">H15-H12</f>
+        <v>10</v>
+      </c>
+      <c r="H14" s="19" t="n">
+        <f aca="false">P12-H12</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="17" t="n">
         <f aca="false">H6</f>
         <v>3</v>
       </c>
-      <c r="Q14" s="16"/>
-      <c r="R14" s="17"/>
-      <c r="S14" s="19"/>
-      <c r="T14" s="21"/>
-      <c r="U14" s="15" t="n">
+      <c r="Q14" s="18" t="n">
+        <f aca="false">R15-R12</f>
+        <v>10</v>
+      </c>
+      <c r="R14" s="19" t="n">
+        <f aca="false">U12-R12</f>
+        <v>10</v>
+      </c>
+      <c r="S14" s="23"/>
+      <c r="T14" s="25"/>
+      <c r="U14" s="17" t="n">
         <f aca="false">H7</f>
         <v>3</v>
       </c>
-      <c r="V14" s="16"/>
-      <c r="W14" s="17"/>
-      <c r="X14" s="19"/>
-      <c r="Y14" s="19"/>
-      <c r="Z14" s="15" t="n">
+      <c r="V14" s="18" t="n">
+        <f aca="false">W15-W12</f>
+        <v>0</v>
+      </c>
+      <c r="W14" s="19" t="n">
+        <f aca="false">Z12-W12</f>
+        <v>0</v>
+      </c>
+      <c r="X14" s="23"/>
+      <c r="Y14" s="23"/>
+      <c r="Z14" s="17" t="n">
         <f aca="false">H9</f>
         <v>9</v>
       </c>
-      <c r="AA14" s="16"/>
-      <c r="AB14" s="17"/>
+      <c r="AA14" s="18" t="n">
+        <f aca="false">AB15-AB12</f>
+        <v>0</v>
+      </c>
+      <c r="AB14" s="19"/>
       <c r="AC14" s="4"/>
       <c r="AD14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="22"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="24"/>
+      <c r="A15" s="20" t="n">
+        <f aca="false">C15-A14</f>
+        <v>0</v>
+      </c>
+      <c r="B15" s="11"/>
+      <c r="C15" s="16" t="n">
+        <f aca="false">MIN(F15,F21)</f>
+        <v>6</v>
+      </c>
+      <c r="D15" s="26"/>
       <c r="E15" s="4"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="23"/>
+      <c r="F15" s="20" t="n">
+        <f aca="false">H15-F14</f>
+        <v>16</v>
+      </c>
+      <c r="G15" s="11"/>
+      <c r="H15" s="16" t="n">
+        <f aca="false">P15</f>
+        <v>23</v>
+      </c>
       <c r="I15" s="4"/>
       <c r="O15" s="4"/>
-      <c r="P15" s="22"/>
-      <c r="Q15" s="12"/>
-      <c r="R15" s="23"/>
+      <c r="P15" s="20" t="n">
+        <f aca="false">R15-P14</f>
+        <v>23</v>
+      </c>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="16" t="n">
+        <f aca="false">U15</f>
+        <v>26</v>
+      </c>
       <c r="S15" s="4"/>
-      <c r="T15" s="25"/>
-      <c r="U15" s="22"/>
-      <c r="V15" s="12"/>
-      <c r="W15" s="23"/>
+      <c r="T15" s="27"/>
+      <c r="U15" s="20" t="n">
+        <f aca="false">W15-U14</f>
+        <v>26</v>
+      </c>
+      <c r="V15" s="11"/>
+      <c r="W15" s="16" t="n">
+        <f aca="false">Z15</f>
+        <v>29</v>
+      </c>
       <c r="X15" s="4"/>
       <c r="Y15" s="4"/>
-      <c r="Z15" s="22"/>
-      <c r="AA15" s="12"/>
-      <c r="AB15" s="23"/>
+      <c r="Z15" s="20" t="n">
+        <f aca="false">AB15-Z14</f>
+        <v>29</v>
+      </c>
+      <c r="AA15" s="11"/>
+      <c r="AB15" s="16" t="n">
+        <f aca="false">AB12</f>
+        <v>38</v>
+      </c>
       <c r="AC15" s="4"/>
       <c r="AD15" s="4"/>
     </row>
@@ -1620,87 +1796,141 @@
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
-      <c r="D16" s="26"/>
-      <c r="T16" s="27"/>
+      <c r="D16" s="28"/>
+      <c r="T16" s="29"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
-      <c r="D17" s="26"/>
-      <c r="T17" s="27"/>
+      <c r="D17" s="28"/>
+      <c r="T17" s="29"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="26"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="13"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="13"/>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="12"/>
-      <c r="R18" s="13"/>
-      <c r="T18" s="27"/>
+      <c r="D18" s="28"/>
+      <c r="F18" s="5" t="n">
+        <f aca="false">C12</f>
+        <v>6</v>
+      </c>
+      <c r="G18" s="11"/>
+      <c r="H18" s="12" t="n">
+        <f aca="false">F18+F20</f>
+        <v>10</v>
+      </c>
+      <c r="K18" s="5" t="n">
+        <f aca="false">H18</f>
+        <v>10</v>
+      </c>
+      <c r="L18" s="11"/>
+      <c r="M18" s="12" t="n">
+        <f aca="false">K18+K20</f>
+        <v>19</v>
+      </c>
+      <c r="P18" s="5" t="n">
+        <f aca="false">M18</f>
+        <v>19</v>
+      </c>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="12" t="n">
+        <f aca="false">P18+P20</f>
+        <v>26</v>
+      </c>
+      <c r="T18" s="29"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D19" s="26"/>
-      <c r="F19" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="K19" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="P19" s="14" t="s">
+      <c r="D19" s="28"/>
+      <c r="F19" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="Q19" s="14"/>
-      <c r="R19" s="14"/>
-      <c r="T19" s="27"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="K19" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="P19" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="15"/>
+      <c r="T19" s="29"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E20" s="19"/>
-      <c r="F20" s="15" t="n">
+      <c r="E20" s="23"/>
+      <c r="F20" s="17" t="n">
         <f aca="false">H4</f>
         <v>4</v>
       </c>
-      <c r="G20" s="16"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="15" t="n">
+      <c r="G20" s="18" t="n">
+        <f aca="false">H21-H18</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="19" t="n">
+        <f aca="false">K18-H18</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="17" t="n">
         <f aca="false">H5</f>
         <v>9</v>
       </c>
-      <c r="L20" s="16"/>
-      <c r="M20" s="17"/>
-      <c r="N20" s="19"/>
-      <c r="O20" s="19"/>
-      <c r="P20" s="15" t="n">
+      <c r="L20" s="18" t="n">
+        <f aca="false">M21-M18</f>
+        <v>0</v>
+      </c>
+      <c r="M20" s="19" t="n">
+        <f aca="false">P18-M18</f>
+        <v>0</v>
+      </c>
+      <c r="N20" s="23"/>
+      <c r="O20" s="23"/>
+      <c r="P20" s="17" t="n">
         <f aca="false">H8</f>
         <v>7</v>
       </c>
-      <c r="Q20" s="16"/>
-      <c r="R20" s="17"/>
-      <c r="S20" s="19"/>
+      <c r="Q20" s="18" t="n">
+        <f aca="false">R21-R18</f>
+        <v>0</v>
+      </c>
+      <c r="R20" s="19" t="n">
+        <f aca="false">U12-R18</f>
+        <v>0</v>
+      </c>
+      <c r="S20" s="23"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F21" s="22"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="23"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="23"/>
-      <c r="P21" s="22"/>
-      <c r="Q21" s="12"/>
-      <c r="R21" s="23"/>
+      <c r="F21" s="20" t="n">
+        <f aca="false">H21-F20</f>
+        <v>6</v>
+      </c>
+      <c r="G21" s="11"/>
+      <c r="H21" s="16" t="n">
+        <f aca="false">K21</f>
+        <v>10</v>
+      </c>
+      <c r="K21" s="20" t="n">
+        <f aca="false">M21-K20</f>
+        <v>10</v>
+      </c>
+      <c r="L21" s="11"/>
+      <c r="M21" s="16" t="n">
+        <f aca="false">P21</f>
+        <v>19</v>
+      </c>
+      <c r="P21" s="20" t="n">
+        <f aca="false">R21-P20</f>
+        <v>19</v>
+      </c>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="16" t="n">
+        <f aca="false">U15</f>
+        <v>26</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4"/>
@@ -1770,141 +2000,148 @@
       <c r="AD30" s="4"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="28" t="s">
-        <v>13</v>
+      <c r="A32" s="30" t="s">
+        <v>4</v>
       </c>
       <c r="B32" s="4"/>
-      <c r="C32" s="29" t="s">
+      <c r="C32" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="33"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="32"/>
+      <c r="I34" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="J34" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="K34" s="32"/>
+      <c r="L34" s="32"/>
+      <c r="M34" s="32"/>
+      <c r="N34" s="32"/>
+      <c r="O34" s="32"/>
+      <c r="P34" s="32"/>
+      <c r="Q34" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="R34" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="S34" s="32"/>
+      <c r="T34" s="32"/>
+      <c r="U34" s="32"/>
+      <c r="V34" s="32"/>
+      <c r="W34" s="32"/>
+      <c r="X34" s="32"/>
+      <c r="Y34" s="32"/>
+      <c r="Z34" s="32"/>
+      <c r="AA34" s="32"/>
+      <c r="AB34" s="32"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" s="4"/>
+      <c r="C35" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="D32" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="E32" s="30"/>
-      <c r="F32" s="30"/>
-      <c r="G32" s="30"/>
-      <c r="H32" s="30"/>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E33" s="30"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="30"/>
-    </row>
-    <row r="34" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="B34" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="C34" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="D34" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="J34" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="K34" s="30"/>
-      <c r="L34" s="30"/>
-      <c r="M34" s="30"/>
-      <c r="N34" s="30"/>
-      <c r="O34" s="30"/>
-      <c r="P34" s="30"/>
-      <c r="Q34" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="R34" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="S34" s="30"/>
-      <c r="T34" s="30"/>
-      <c r="U34" s="30"/>
-      <c r="V34" s="30"/>
-      <c r="W34" s="30"/>
-      <c r="X34" s="30"/>
-      <c r="Y34" s="30"/>
-      <c r="Z34" s="30"/>
-      <c r="AA34" s="30"/>
-      <c r="AB34" s="30"/>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="D35" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="E35" s="30"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="30"/>
-      <c r="H35" s="30"/>
+      <c r="D35" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="32"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="C36" s="38" t="s">
-        <v>28</v>
+      <c r="A36" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="40" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="38"/>
-      <c r="C37" s="38"/>
+      <c r="A37" s="40"/>
+      <c r="C37" s="40"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="38"/>
-      <c r="C38" s="38"/>
+      <c r="A38" s="40"/>
+      <c r="C38" s="40"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="38"/>
-      <c r="C39" s="38"/>
+      <c r="A39" s="40"/>
+      <c r="C39" s="40"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="38"/>
-      <c r="C40" s="38"/>
+      <c r="A40" s="40"/>
+      <c r="C40" s="40"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="38"/>
-      <c r="C41" s="38"/>
+      <c r="A41" s="40"/>
+      <c r="C41" s="40"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="38"/>
-      <c r="C42" s="38"/>
+      <c r="A42" s="40"/>
+      <c r="C42" s="40"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="38"/>
-      <c r="C43" s="38"/>
+      <c r="A43" s="40"/>
+      <c r="C43" s="40"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="38"/>
-      <c r="C44" s="38"/>
+      <c r="A44" s="40"/>
+      <c r="C44" s="40"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="26">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
+    <mergeCell ref="Q1:W1"/>
+    <mergeCell ref="Q2:W2"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="Q3:W3"/>
+    <mergeCell ref="Q4:W4"/>
+    <mergeCell ref="Q5:W5"/>
+    <mergeCell ref="Q6:W6"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="F13:H13"/>
     <mergeCell ref="P13:R13"/>
@@ -1928,7 +2165,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B14 G14 G20 L20 Q14 Q20 V14 AA14">
+  <conditionalFormatting sqref="AA14 L4 O5 V14 Q14 Q20 L20 G20 G14 B14">
     <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>0</formula>
     </cfRule>
@@ -1950,87 +2187,87 @@
   </sheetPr>
   <dimension ref="A1:R63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P9" activeCellId="0" sqref="P9:R12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P9" activeCellId="0" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="35" width="3.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="37" width="3.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="41" t="s">
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="39" t="s">
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="41" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="8"/>
+      <c r="B2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="10"/>
       <c r="H2" s="1" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
       <c r="H3" s="1" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="8" t="s">
+      <c r="C4" s="10"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
       <c r="H4" s="1" t="n">
         <v>4</v>
       </c>
@@ -2039,382 +2276,382 @@
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="8" t="s">
+      <c r="B5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
+      <c r="C5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
       <c r="H5" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
       <c r="H6" s="1" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="n">
+      <c r="A9" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="13"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="13"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="13"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="13"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="12"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="12"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="12"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="F10" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="K10" s="14" t="s">
+      <c r="A10" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="F10" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="K10" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="P10" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q10" s="14"/>
-      <c r="R10" s="14"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="P10" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="15" t="n">
+      <c r="A11" s="17" t="n">
         <f aca="false" t="array" ref="A11:A11">VLOOKUP(A10,$A$2:$H$10,8)</f>
         <v>6</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="17"/>
-      <c r="F11" s="15" t="n">
+      <c r="B11" s="18"/>
+      <c r="C11" s="19"/>
+      <c r="F11" s="17" t="n">
         <f aca="false" t="array" ref="F11:F11">VLOOKUP(F10,$A$2:$H$10,8)</f>
         <v>7</v>
       </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="17"/>
-      <c r="K11" s="15" t="n">
+      <c r="G11" s="18"/>
+      <c r="H11" s="19"/>
+      <c r="K11" s="17" t="n">
         <f aca="false" t="array" ref="K11:K11">VLOOKUP(K10,$A$2:$H$10,8)</f>
         <v>5</v>
       </c>
-      <c r="L11" s="16"/>
-      <c r="M11" s="17"/>
-      <c r="P11" s="15" t="n">
+      <c r="L11" s="18"/>
+      <c r="M11" s="19"/>
+      <c r="P11" s="17" t="n">
         <f aca="false" t="array" ref="P11:P11">VLOOKUP(P10,$A$2:$H$10,8)</f>
         <v>9</v>
       </c>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="17"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="19"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="22"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="23"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="23"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="23"/>
-      <c r="P12" s="22"/>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="23"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="16"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="16"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="16"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="16"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F15" s="11"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="13"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="12"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F16" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
+      <c r="F16" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F17" s="15" t="n">
+      <c r="F17" s="17" t="n">
         <f aca="false" t="array" ref="F17:F17">VLOOKUP(F16,$A$2:$H$10,8)</f>
         <v>4</v>
       </c>
-      <c r="G17" s="16"/>
-      <c r="H17" s="17"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="19"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F18" s="22"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="23"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="16"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="42"/>
-      <c r="B50" s="43"/>
-      <c r="C50" s="43"/>
-      <c r="D50" s="43"/>
-      <c r="E50" s="43"/>
-      <c r="F50" s="43"/>
-      <c r="G50" s="43"/>
-      <c r="H50" s="43"/>
-      <c r="I50" s="43"/>
-      <c r="J50" s="43"/>
-      <c r="K50" s="43"/>
-      <c r="L50" s="43"/>
+      <c r="A50" s="44"/>
+      <c r="B50" s="45"/>
+      <c r="C50" s="45"/>
+      <c r="D50" s="45"/>
+      <c r="E50" s="45"/>
+      <c r="F50" s="45"/>
+      <c r="G50" s="45"/>
+      <c r="H50" s="45"/>
+      <c r="I50" s="45"/>
+      <c r="J50" s="45"/>
+      <c r="K50" s="45"/>
+      <c r="L50" s="45"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="42"/>
-      <c r="B51" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="C51" s="44"/>
-      <c r="D51" s="44" t="s">
+      <c r="A51" s="44"/>
+      <c r="B51" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="C51" s="46"/>
+      <c r="D51" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="46"/>
+      <c r="F51" s="46"/>
+      <c r="G51" s="46"/>
+      <c r="H51" s="46"/>
+      <c r="I51" s="46"/>
+      <c r="J51" s="46"/>
+      <c r="K51" s="46"/>
+      <c r="L51" s="45"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="44"/>
+      <c r="B52" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" s="47"/>
+      <c r="D52" s="47"/>
+      <c r="E52" s="46"/>
+      <c r="F52" s="48" t="s">
+        <v>36</v>
+      </c>
+      <c r="G52" s="48"/>
+      <c r="H52" s="48"/>
+      <c r="I52" s="48"/>
+      <c r="J52" s="48"/>
+      <c r="K52" s="46"/>
+      <c r="L52" s="45"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="44"/>
+      <c r="B53" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53" s="50" t="s">
+        <v>17</v>
+      </c>
+      <c r="D53" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="E53" s="46"/>
+      <c r="F53" s="46"/>
+      <c r="G53" s="46"/>
+      <c r="H53" s="46"/>
+      <c r="I53" s="46"/>
+      <c r="J53" s="46"/>
+      <c r="K53" s="46"/>
+      <c r="L53" s="45"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="44"/>
+      <c r="B54" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="C54" s="46"/>
+      <c r="D54" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="E51" s="44"/>
-      <c r="F51" s="44"/>
-      <c r="G51" s="44"/>
-      <c r="H51" s="44"/>
-      <c r="I51" s="44"/>
-      <c r="J51" s="44"/>
-      <c r="K51" s="44"/>
-      <c r="L51" s="43"/>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="42"/>
-      <c r="B52" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="C52" s="45"/>
-      <c r="D52" s="45"/>
-      <c r="E52" s="44"/>
-      <c r="F52" s="46" t="s">
-        <v>29</v>
-      </c>
-      <c r="G52" s="46"/>
-      <c r="H52" s="46"/>
-      <c r="I52" s="46"/>
-      <c r="J52" s="46"/>
-      <c r="K52" s="44"/>
-      <c r="L52" s="43"/>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="42"/>
-      <c r="B53" s="47" t="s">
+      <c r="E54" s="46"/>
+      <c r="F54" s="46"/>
+      <c r="G54" s="46"/>
+      <c r="H54" s="46"/>
+      <c r="I54" s="46"/>
+      <c r="J54" s="46"/>
+      <c r="K54" s="46"/>
+      <c r="L54" s="45"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="44"/>
+      <c r="B55" s="46"/>
+      <c r="C55" s="46"/>
+      <c r="D55" s="46"/>
+      <c r="E55" s="46"/>
+      <c r="F55" s="46"/>
+      <c r="G55" s="46"/>
+      <c r="H55" s="46"/>
+      <c r="I55" s="46"/>
+      <c r="J55" s="46"/>
+      <c r="K55" s="46"/>
+      <c r="L55" s="45"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="44"/>
+      <c r="B56" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="C56" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="D56" s="52"/>
+      <c r="E56" s="52"/>
+      <c r="F56" s="52"/>
+      <c r="G56" s="52"/>
+      <c r="H56" s="52"/>
+      <c r="I56" s="52"/>
+      <c r="J56" s="52"/>
+      <c r="K56" s="52"/>
+      <c r="L56" s="45"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="44"/>
+      <c r="B57" s="51" t="s">
+        <v>19</v>
+      </c>
+      <c r="C57" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="D57" s="52"/>
+      <c r="E57" s="52"/>
+      <c r="F57" s="52"/>
+      <c r="G57" s="52"/>
+      <c r="H57" s="52"/>
+      <c r="I57" s="52"/>
+      <c r="J57" s="52"/>
+      <c r="K57" s="52"/>
+      <c r="L57" s="45"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="44"/>
+      <c r="B58" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="C58" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="D58" s="52"/>
+      <c r="E58" s="52"/>
+      <c r="F58" s="52"/>
+      <c r="G58" s="52"/>
+      <c r="H58" s="52"/>
+      <c r="I58" s="52"/>
+      <c r="J58" s="52"/>
+      <c r="K58" s="52"/>
+      <c r="L58" s="45"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="44"/>
+      <c r="B59" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="C59" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="D59" s="52"/>
+      <c r="E59" s="52"/>
+      <c r="F59" s="52"/>
+      <c r="G59" s="52"/>
+      <c r="H59" s="52"/>
+      <c r="I59" s="52"/>
+      <c r="J59" s="52"/>
+      <c r="K59" s="52"/>
+      <c r="L59" s="45"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="44"/>
+      <c r="B60" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="C53" s="48" t="s">
+      <c r="C60" s="52" t="s">
+        <v>41</v>
+      </c>
+      <c r="D60" s="52"/>
+      <c r="E60" s="52"/>
+      <c r="F60" s="52"/>
+      <c r="G60" s="52"/>
+      <c r="H60" s="52"/>
+      <c r="I60" s="52"/>
+      <c r="J60" s="52"/>
+      <c r="K60" s="52"/>
+      <c r="L60" s="45"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="44"/>
+      <c r="B61" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="D53" s="47" t="s">
+      <c r="C61" s="52" t="s">
+        <v>42</v>
+      </c>
+      <c r="D61" s="52"/>
+      <c r="E61" s="52"/>
+      <c r="F61" s="52"/>
+      <c r="G61" s="52"/>
+      <c r="H61" s="52"/>
+      <c r="I61" s="52"/>
+      <c r="J61" s="52"/>
+      <c r="K61" s="52"/>
+      <c r="L61" s="45"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="44"/>
+      <c r="B62" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="E53" s="44"/>
-      <c r="F53" s="44"/>
-      <c r="G53" s="44"/>
-      <c r="H53" s="44"/>
-      <c r="I53" s="44"/>
-      <c r="J53" s="44"/>
-      <c r="K53" s="44"/>
-      <c r="L53" s="43"/>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="42"/>
-      <c r="B54" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="C54" s="44"/>
-      <c r="D54" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="E54" s="44"/>
-      <c r="F54" s="44"/>
-      <c r="G54" s="44"/>
-      <c r="H54" s="44"/>
-      <c r="I54" s="44"/>
-      <c r="J54" s="44"/>
-      <c r="K54" s="44"/>
-      <c r="L54" s="43"/>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="42"/>
-      <c r="B55" s="44"/>
-      <c r="C55" s="44"/>
-      <c r="D55" s="44"/>
-      <c r="E55" s="44"/>
-      <c r="F55" s="44"/>
-      <c r="G55" s="44"/>
-      <c r="H55" s="44"/>
-      <c r="I55" s="44"/>
-      <c r="J55" s="44"/>
-      <c r="K55" s="44"/>
-      <c r="L55" s="43"/>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="42"/>
-      <c r="B56" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="C56" s="50" t="s">
-        <v>30</v>
-      </c>
-      <c r="D56" s="50"/>
-      <c r="E56" s="50"/>
-      <c r="F56" s="50"/>
-      <c r="G56" s="50"/>
-      <c r="H56" s="50"/>
-      <c r="I56" s="50"/>
-      <c r="J56" s="50"/>
-      <c r="K56" s="50"/>
-      <c r="L56" s="43"/>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="42"/>
-      <c r="B57" s="49" t="s">
-        <v>24</v>
-      </c>
-      <c r="C57" s="50" t="s">
-        <v>31</v>
-      </c>
-      <c r="D57" s="50"/>
-      <c r="E57" s="50"/>
-      <c r="F57" s="50"/>
-      <c r="G57" s="50"/>
-      <c r="H57" s="50"/>
-      <c r="I57" s="50"/>
-      <c r="J57" s="50"/>
-      <c r="K57" s="50"/>
-      <c r="L57" s="43"/>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="42"/>
-      <c r="B58" s="49" t="s">
-        <v>14</v>
-      </c>
-      <c r="C58" s="50" t="s">
-        <v>32</v>
-      </c>
-      <c r="D58" s="50"/>
-      <c r="E58" s="50"/>
-      <c r="F58" s="50"/>
-      <c r="G58" s="50"/>
-      <c r="H58" s="50"/>
-      <c r="I58" s="50"/>
-      <c r="J58" s="50"/>
-      <c r="K58" s="50"/>
-      <c r="L58" s="43"/>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="42"/>
-      <c r="B59" s="49" t="s">
-        <v>25</v>
-      </c>
-      <c r="C59" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="D59" s="50"/>
-      <c r="E59" s="50"/>
-      <c r="F59" s="50"/>
-      <c r="G59" s="50"/>
-      <c r="H59" s="50"/>
-      <c r="I59" s="50"/>
-      <c r="J59" s="50"/>
-      <c r="K59" s="50"/>
-      <c r="L59" s="43"/>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="42"/>
-      <c r="B60" s="47" t="s">
-        <v>3</v>
-      </c>
-      <c r="C60" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="D60" s="50"/>
-      <c r="E60" s="50"/>
-      <c r="F60" s="50"/>
-      <c r="G60" s="50"/>
-      <c r="H60" s="50"/>
-      <c r="I60" s="50"/>
-      <c r="J60" s="50"/>
-      <c r="K60" s="50"/>
-      <c r="L60" s="43"/>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="42"/>
-      <c r="B61" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="C61" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="D61" s="50"/>
-      <c r="E61" s="50"/>
-      <c r="F61" s="50"/>
-      <c r="G61" s="50"/>
-      <c r="H61" s="50"/>
-      <c r="I61" s="50"/>
-      <c r="J61" s="50"/>
-      <c r="K61" s="50"/>
-      <c r="L61" s="43"/>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="42"/>
-      <c r="B62" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="C62" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="D62" s="43"/>
-      <c r="E62" s="43"/>
-      <c r="F62" s="43"/>
-      <c r="G62" s="43"/>
-      <c r="H62" s="43"/>
-      <c r="I62" s="43"/>
-      <c r="J62" s="43"/>
-      <c r="K62" s="43"/>
-      <c r="L62" s="43"/>
+      <c r="C62" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="D62" s="45"/>
+      <c r="E62" s="45"/>
+      <c r="F62" s="45"/>
+      <c r="G62" s="45"/>
+      <c r="H62" s="45"/>
+      <c r="I62" s="45"/>
+      <c r="J62" s="45"/>
+      <c r="K62" s="45"/>
+      <c r="L62" s="45"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="42"/>
-      <c r="B63" s="43"/>
-      <c r="C63" s="43"/>
-      <c r="D63" s="43"/>
-      <c r="E63" s="43"/>
-      <c r="F63" s="43"/>
-      <c r="G63" s="43"/>
-      <c r="H63" s="43"/>
-      <c r="I63" s="43"/>
-      <c r="J63" s="43"/>
-      <c r="K63" s="43"/>
-      <c r="L63" s="43"/>
+      <c r="A63" s="44"/>
+      <c r="B63" s="45"/>
+      <c r="C63" s="45"/>
+      <c r="D63" s="45"/>
+      <c r="E63" s="45"/>
+      <c r="F63" s="45"/>
+      <c r="G63" s="45"/>
+      <c r="H63" s="45"/>
+      <c r="I63" s="45"/>
+      <c r="J63" s="45"/>
+      <c r="K63" s="45"/>
+      <c r="L63" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="15">

</xml_diff>